<commit_message>
Gruppenvertrag hinzugefügt, Zeitplan Zwischenpräsi eingefügt
</commit_message>
<xml_diff>
--- a/Documentation/Zeitplan.xlsx
+++ b/Documentation/Zeitplan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeit\semester5\bacherlorVorbereitung\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Arbeit\semester5\bacherlorVorbereitung\BachelorStudyProject\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FED5510-19D0-4440-909D-DD69290408BE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83042CBE-4306-490C-9B9F-5CF4905872E9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="593" xr2:uid="{6E8C514B-258B-4C42-9507-A0318310B1C4}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Aufgaben/Zeit</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>LevelDesign</t>
+  </si>
+  <si>
+    <t>Zwischen Präsentation</t>
   </si>
 </sst>
 </file>
@@ -556,9 +559,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6C12F2-6480-4BB7-B246-B8F09C17CDF6}">
   <dimension ref="A1:EX35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DD40" sqref="DD40"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BA1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A29" sqref="A29:A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -567,6 +570,7 @@
     <col min="31" max="31" width="29.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="25.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="71" max="71" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="19.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="105" max="105" width="22.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="120" max="130" width="11.5546875" style="9"/>
   </cols>
@@ -806,7 +810,7 @@
       <c r="BZ1" s="1">
         <v>43570</v>
       </c>
-      <c r="CA1" s="1">
+      <c r="CA1" s="7">
         <v>43571</v>
       </c>
       <c r="CB1" s="1">
@@ -1001,6 +1005,9 @@
       <c r="BS2" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="CA2" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="DA2" s="2" t="s">
         <v>38</v>
       </c>
@@ -1190,7 +1197,6 @@
       <c r="BX20" s="5"/>
       <c r="BY20" s="5"/>
       <c r="BZ20" s="5"/>
-      <c r="CA20" s="5"/>
       <c r="CB20" s="5"/>
       <c r="CC20" s="5"/>
       <c r="CD20" s="5"/>

</xml_diff>